<commit_message>
Clean up on-failure error reporting
</commit_message>
<xml_diff>
--- a/form-files/framework/default.xlsx
+++ b/form-files/framework/default.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="564" windowWidth="23256" windowHeight="12372"/>
+    <workbookView xWindow="230" yWindow="560" windowWidth="23260" windowHeight="12370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
     <sheet name="survey" sheetId="1" r:id="rId2"/>
     <sheet name="settings" sheetId="4" r:id="rId3"/>
+    <sheet name="choices" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
   <si>
     <t>comments</t>
   </si>
@@ -79,6 +80,132 @@
   </si>
   <si>
     <t>display.title</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>opendatakit.getPlatformInfo().container == "Chrome"</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>user_branch</t>
+  </si>
+  <si>
+    <t>choice_list_name</t>
+  </si>
+  <si>
+    <t>data_value</t>
+  </si>
+  <si>
+    <t>test_forms</t>
+  </si>
+  <si>
+    <t>breathcounter</t>
+  </si>
+  <si>
+    <t>customAppearance</t>
+  </si>
+  <si>
+    <t>exampleForm</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>household_new</t>
+  </si>
+  <si>
+    <t>household_member</t>
+  </si>
+  <si>
+    <t>imnci_test</t>
+  </si>
+  <si>
+    <t>refrigerators_init</t>
+  </si>
+  <si>
+    <t>refrigerators_update</t>
+  </si>
+  <si>
+    <t>section_test</t>
+  </si>
+  <si>
+    <t>selects</t>
+  </si>
+  <si>
+    <t>branch_label</t>
+  </si>
+  <si>
+    <t>values_list</t>
+  </si>
+  <si>
+    <t>Choose a test form</t>
+  </si>
+  <si>
+    <t>exit section</t>
+  </si>
+  <si>
+    <t>external_link</t>
+  </si>
+  <si>
+    <t>Open form</t>
+  </si>
+  <si>
+    <t>url.cell_type</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/breathcounter/forms/breathcounter/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/complex_validate_test/forms/complex_validate_test/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/customAppearance/forms/customAppearance/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/exampleForm/forms/exampleForm/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/household/forms/household/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/household/forms/household_new/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/household_member/forms/household_member/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/refrigerators/forms/refrigerators_update/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/refrigerators/forms/refrigerators_init/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/imnci/forms/imnci_test/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/section_test/forms/section_test/',null)</t>
+  </si>
+  <si>
+    <t>opendatakit.getHashString('../tables/selects/forms/selects/',null)</t>
+  </si>
+  <si>
+    <t>complex_validate_test</t>
   </si>
 </sst>
 </file>
@@ -117,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -127,6 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,17 +558,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" ht="19.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -460,88 +588,465 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="17.08984375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="2" max="2" width="28.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="5" max="5" width="46.08984375" customWidth="1"/>
+    <col min="6" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" customWidth="1"/>
+    <col min="9" max="9" width="31.453125" customWidth="1"/>
+    <col min="10" max="10" width="22.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="b">
+      <c r="J5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="4" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="5" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="6" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="7" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="8" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="9" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="10" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="11" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="12" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="13" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="14" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="15" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="16" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="18" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="19" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="20" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="21" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="22" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="23" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="24" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="25" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="26" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="27" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="28" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="29" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="30" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="31" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="32" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="33" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="34" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="35" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="36" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="37" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="38" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="39" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="40" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="42" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="43" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="44" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" t="s">
+        <v>45</v>
+      </c>
+      <c r="H42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -552,16 +1057,16 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="17.08984375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" customWidth="1"/>
+    <col min="4" max="4" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -575,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -587,7 +1092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -598,7 +1103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -609,61 +1114,224 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="8" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="9" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change 'logic_flow' to 'specification' in generated JSON
</commit_message>
<xml_diff>
--- a/form-files/framework/default.xlsx
+++ b/form-files/framework/default.xlsx
@@ -590,13 +590,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.08984375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.36328125" customWidth="1"/>
+    <col min="2" max="2" width="88.7265625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="22.26953125" customWidth="1"/>
     <col min="5" max="5" width="46.08984375" customWidth="1"/>

</xml_diff>